<commit_message>
Export excel students, change view client
</commit_message>
<xml_diff>
--- a/public/management-assets/template/import_student_template.xlsx
+++ b/public/management-assets/template/import_student_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\autocareerbridge\public\storage\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\autocareerbridge\public\management-assets\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38547D10-BF0B-4CF3-B820-AD1CFBBE5FA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{321ECC70-0573-40D9-AAF1-22F02E56AEDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27840" yWindow="3720" windowWidth="21600" windowHeight="11235" xr2:uid="{7C5960F5-9DF4-4ACF-9728-BC3AB00EA6AE}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7C5960F5-9DF4-4ACF-9728-BC3AB00EA6AE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -48,38 +48,122 @@
     <t>0920233873</t>
   </si>
   <si>
-    <t>Mã sinh viên</t>
-  </si>
-  <si>
-    <t>Tên chuyên ngành</t>
-  </si>
-  <si>
-    <t>Họ và tên sinh viên</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Số điện thoại</t>
-  </si>
-  <si>
-    <t>Giới tính (nam hoặc nữ)</t>
-  </si>
-  <si>
-    <t>Ngày nhập học</t>
-  </si>
-  <si>
     <t>Ngày ra trường</t>
   </si>
   <si>
     <t>Mô tả</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Mã sinh viên </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Tên chuyên ngành </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Họ và tên sinh viên </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Email </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Số điện thoại </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Giới tính (nam hoặc nữ) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ngày nhập học </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -95,6 +179,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -451,7 +542,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -469,31 +560,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Add skill to students and multi lang daterange
</commit_message>
<xml_diff>
--- a/public/management-assets/template/import_student_template.xlsx
+++ b/public/management-assets/template/import_student_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\autocareerbridge\public\management-assets\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{321ECC70-0573-40D9-AAF1-22F02E56AEDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB2F272B-5EDE-4017-81F2-163A7F2AE5E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7C5960F5-9DF4-4ACF-9728-BC3AB00EA6AE}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>mô tả</t>
   </si>
@@ -157,6 +157,12 @@
       </rPr>
       <t>*</t>
     </r>
+  </si>
+  <si>
+    <t>Kỹ năng</t>
+  </si>
+  <si>
+    <t>php, laravel</t>
   </si>
 </sst>
 </file>
@@ -539,10 +545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EED285B3-A023-428D-83C1-ADD665ECA36F}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -554,11 +560,11 @@
     <col min="5" max="5" width="16.5546875" style="2" customWidth="1"/>
     <col min="6" max="6" width="24.109375" customWidth="1"/>
     <col min="7" max="7" width="19" customWidth="1"/>
-    <col min="8" max="8" width="17" customWidth="1"/>
-    <col min="9" max="9" width="14.77734375" customWidth="1"/>
+    <col min="8" max="9" width="17" customWidth="1"/>
+    <col min="10" max="10" width="14.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -583,11 +589,14 @@
       <c r="H1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -612,7 +621,10 @@
       <c r="H2" s="3">
         <v>45332</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>